<commit_message>
added mp3 and wav
</commit_message>
<xml_diff>
--- a/EntrTest.xlsx
+++ b/EntrTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t xml:space="preserve">Videos </t>
   </si>
@@ -27,9 +27,6 @@
     <t>File Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Entropy </t>
-  </si>
-  <si>
     <t>Sample1.avi</t>
   </si>
   <si>
@@ -91,6 +88,42 @@
   </si>
   <si>
     <t>mp3</t>
+  </si>
+  <si>
+    <t>Sample1.mp3</t>
+  </si>
+  <si>
+    <t>Sample2.mp3</t>
+  </si>
+  <si>
+    <t>Sample3.mp3</t>
+  </si>
+  <si>
+    <t>Sample4.mp3</t>
+  </si>
+  <si>
+    <t>Sample5.mp3</t>
+  </si>
+  <si>
+    <t>wav</t>
+  </si>
+  <si>
+    <t>Sample1.wav</t>
+  </si>
+  <si>
+    <t>Sample2.wav</t>
+  </si>
+  <si>
+    <t>Sample3.wav</t>
+  </si>
+  <si>
+    <t>Sample4.wav</t>
+  </si>
+  <si>
+    <t>Sample5.wav</t>
+  </si>
+  <si>
+    <t>Entropy (%)</t>
   </si>
 </sst>
 </file>
@@ -141,9 +174,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,22 +481,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -473,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -484,33 +521,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>38709642</v>
@@ -519,7 +556,7 @@
         <v>99.629493999999994</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1">
         <v>16658293</v>
@@ -528,7 +565,7 @@
         <v>99.980521999999993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="1">
         <v>87087</v>
@@ -539,7 +576,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>17639654</v>
@@ -548,7 +585,7 @@
         <v>99.850845000000007</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1">
         <v>16094941</v>
@@ -557,7 +594,7 @@
         <v>99.976234000000005</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="1">
         <v>67644</v>
@@ -568,7 +605,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>10713088</v>
@@ -577,7 +614,7 @@
         <v>99.676902999999996</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1">
         <v>26246048</v>
@@ -586,7 +623,7 @@
         <v>99.885611999999995</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="1">
         <v>42798</v>
@@ -597,7 +634,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>19992576</v>
@@ -606,7 +643,7 @@
         <v>99.806304999999995</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1">
         <v>14117113</v>
@@ -615,7 +652,7 @@
         <v>99.997153999999995</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="1">
         <v>56345</v>
@@ -626,7 +663,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>6410240</v>
@@ -635,7 +672,7 @@
         <v>99.676406999999998</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1">
         <v>4124170</v>
@@ -644,7 +681,7 @@
         <v>99.984504999999999</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="1">
         <v>49676</v>
@@ -654,21 +691,151 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B17" s="1">
+        <v>204029</v>
+      </c>
+      <c r="C17" s="1">
+        <v>98.923232999999996</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="1">
+        <v>491516</v>
+      </c>
+      <c r="G17" s="1">
+        <v>84.951340000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1">
+        <v>722304</v>
+      </c>
+      <c r="C18" s="1">
+        <v>98.165497000000002</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="1">
+        <v>331108</v>
+      </c>
+      <c r="G18" s="1">
+        <v>71.919235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1">
+        <v>9536</v>
+      </c>
+      <c r="C19" s="1">
+        <v>90.644599999999997</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1">
+        <v>355588</v>
+      </c>
+      <c r="G19" s="1">
+        <v>72.179587999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1">
+        <v>86058</v>
+      </c>
+      <c r="C20" s="1">
+        <v>99.093520999999996</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="1">
+        <v>409152</v>
+      </c>
+      <c r="G20" s="1">
+        <v>65.669974999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5408</v>
+      </c>
+      <c r="C21" s="1">
+        <v>87.346275000000006</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="1">
+        <v>728396</v>
+      </c>
+      <c r="G21" s="1">
+        <v>78.855354000000005</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:E11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>